<commit_message>
fix session of sidebar
</commit_message>
<xml_diff>
--- a/@Functions/sofexport.xlsx
+++ b/@Functions/sofexport.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Sheet2" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -41,16 +41,19 @@
     <t>Group</t>
   </si>
   <si>
-    <t>2020-01-01</t>
+    <t>2020-03-17</t>
   </si>
   <si>
-    <t>POC Cont</t>
+    <t>SR2020-03-0698</t>
   </si>
   <si>
-    <t>Strengthening of Peace and Orders Councils</t>
+    <t>To Cover the Payment of Terminal Leave Benefits of Ms. Divinamor T. De Pano</t>
   </si>
   <si>
-    <t>5-02-05-020-01</t>
+    <t>5-01-04-030-01</t>
+  </si>
+  <si>
+    <t>General Management and Supervision</t>
   </si>
   <si>
     <t>For the Conduct of Drug Abuse Treatent and Rehabilitation Center (DATRC) Inter-Agency Task Force Project Management Office (PMO) Site</t>
@@ -194,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -301,21 +304,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="164" fillId="2" borderId="3" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="4" numFmtId="164" fillId="2" borderId="3" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -668,21 +662,21 @@
       <c r="B2" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="37">
-        <v>70</v>
+      <c r="E2" s="36">
+        <v>206416</v>
       </c>
-      <c r="F2" s="38">
-        <v>0</v>
+      <c r="F2" s="37">
+        <v>206415.82</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40" t="s">
-        <v>10</v>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:91">
@@ -1273,7 +1267,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="CM60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:91">
@@ -1286,7 +1280,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="CK61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:91">
@@ -1477,10 +1471,10 @@
       <c r="E80" s="15"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:91" customHeight="1" ht="15">
@@ -1491,10 +1485,10 @@
       <c r="E81" s="15"/>
       <c r="F81" s="29"/>
       <c r="G81" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="82" spans="1:91" customHeight="1" ht="29.25">

</xml_diff>